<commit_message>
Update sample files with ones that work for manual testing. Copied from commit f13ef14
</commit_message>
<xml_diff>
--- a/reconciliation-samples/For debugging/Your-Spreadsheet.xlsx
+++ b/reconciliation-samples/For debugging/Your-Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\reconciliation-samples\For debugging\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF834282-5A80-4E5B-B900-A0BBE2B0D000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4EDA34A-CEDC-43DA-A544-2296E755994D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="6" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Bank In" sheetId="7" r:id="rId1"/>
@@ -257,7 +257,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="121">
   <si>
     <t>notes</t>
   </si>
@@ -319,36 +319,9 @@
     <t>POS</t>
   </si>
   <si>
-    <t>(Intendicles)</t>
-  </si>
-  <si>
     <t>PCL</t>
   </si>
   <si>
-    <t>Description001</t>
-  </si>
-  <si>
-    <t>Description002</t>
-  </si>
-  <si>
-    <t>Description003</t>
-  </si>
-  <si>
-    <t>Description004</t>
-  </si>
-  <si>
-    <t>Description005</t>
-  </si>
-  <si>
-    <t>Description006</t>
-  </si>
-  <si>
-    <t>Description008</t>
-  </si>
-  <si>
-    <t>Description009</t>
-  </si>
-  <si>
     <t>Code</t>
   </si>
   <si>
@@ -478,15 +451,6 @@
     <t>CredCard1 unrecon</t>
   </si>
   <si>
-    <t>!! &lt;-- leftmost column - ActualBank bal recorded from downloaded csv, row "1/10/19, £100, Some Description"</t>
-  </si>
-  <si>
-    <t>!! CredCard2 bal recorded from statement dated Oct 2018</t>
-  </si>
-  <si>
-    <t>!! CredCard1 bal recorded from statement dated Oct 2018</t>
-  </si>
-  <si>
     <t>CredCard1 Balance</t>
   </si>
   <si>
@@ -505,9 +469,6 @@
     <t>new transaction</t>
   </si>
   <si>
-    <t>Description007</t>
-  </si>
-  <si>
     <t>Totals</t>
   </si>
   <si>
@@ -604,15 +565,6 @@
     <t>Annual budgeted amount 003</t>
   </si>
   <si>
-    <t>Bank monthly transaction 01</t>
-  </si>
-  <si>
-    <t>Bank monthly transaction 02</t>
-  </si>
-  <si>
-    <t>Bank monthly transaction 03</t>
-  </si>
-  <si>
     <t>Monthly expense 001</t>
   </si>
   <si>
@@ -623,6 +575,51 @@
   </si>
   <si>
     <t>!! ActualBank bal !!</t>
+  </si>
+  <si>
+    <t>CRED CARD 2</t>
+  </si>
+  <si>
+    <t>"CRED CARD 2"</t>
+  </si>
+  <si>
+    <t>"CRED CARD 1"</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Bank monthly incoming transaction 01</t>
+  </si>
+  <si>
+    <t>Bank monthly incoming transaction 02</t>
+  </si>
+  <si>
+    <t>Bank monthly incoming transaction 03</t>
+  </si>
+  <si>
+    <t>Bank monthly outgoing transaction 01</t>
+  </si>
+  <si>
+    <t>Bank monthly outgoing transaction 02</t>
+  </si>
+  <si>
+    <t>Bank monthly outgoing transaction 03</t>
+  </si>
+  <si>
+    <t>!! CredCard2 bal recorded from statement dated April 2019</t>
+  </si>
+  <si>
+    <t>!! CredCard1 bal recorded from statement dated April 2019</t>
+  </si>
+  <si>
+    <t>!! &lt;-- leftmost column - ActualBank bal recorded from downloaded csv, row "30/4/19, £100, Some Description"</t>
+  </si>
+  <si>
+    <t>CREDIT CARD 1</t>
+  </si>
+  <si>
+    <t>CREDIT CARD 2</t>
   </si>
 </sst>
 </file>
@@ -702,7 +699,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -774,6 +771,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1194,7 +1194,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2:E4"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,17 +1231,17 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>43374</v>
+        <v>43586</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="29" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="13">
@@ -1250,32 +1250,32 @@
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
-      <c r="L2" s="30">
-        <v>43374</v>
+      <c r="L2" s="5">
+        <v>43586</v>
       </c>
       <c r="M2">
         <v>5</v>
       </c>
       <c r="N2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="O2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>43375</v>
+        <v>43587</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3" s="29" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="F3" s="10"/>
       <c r="G3" s="13">
@@ -1284,32 +1284,32 @@
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
-      <c r="L3" s="30">
-        <v>43740</v>
+      <c r="L3" s="5">
+        <v>43587</v>
       </c>
       <c r="M3">
         <v>10</v>
       </c>
       <c r="N3" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="O3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>43376</v>
+        <v>43588</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="29" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="F4" s="10">
         <v>12345</v>
@@ -1320,17 +1320,17 @@
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
-      <c r="L4" s="30">
-        <v>43741</v>
+      <c r="L4" s="5">
+        <v>43588</v>
       </c>
       <c r="M4">
         <v>15</v>
       </c>
       <c r="N4" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="O4" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1341,17 +1341,17 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>43404</v>
+        <v>43616</v>
       </c>
       <c r="B6" s="13">
         <v>5.05</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="7" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="13"/>
@@ -1367,11 +1367,11 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2346053-D1C6-4B74-A036-879FF95C7377}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1384,13 +1384,13 @@
   <sheetData>
     <row r="1" spans="1:11" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="45" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B1" s="34" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D1" s="39"/>
       <c r="E1" s="34" t="s">
@@ -1400,220 +1400,83 @@
         <v>3</v>
       </c>
       <c r="G1" s="34" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="17"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="18">
+        <f>$J$2+K2</f>
+        <v>43617</v>
+      </c>
+      <c r="C2" s="17">
+        <v>21.762</v>
+      </c>
       <c r="D2" s="17"/>
+      <c r="E2" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="J2" s="20">
+        <v>43616</v>
+      </c>
+      <c r="K2" s="14">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:11" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="18">
-        <f>$J$3+K3</f>
-        <v>43405</v>
+        <f>$J$2+K3</f>
+        <v>43618</v>
       </c>
       <c r="C3" s="17">
-        <v>21.762</v>
+        <v>15.600000000000001</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="20">
-        <v>43404</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="J3" s="20"/>
       <c r="K3" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="18">
-        <f t="shared" ref="B4:B10" si="0">$J$3+K4</f>
-        <v>43405</v>
+        <f>$J$2+K4</f>
+        <v>43619</v>
       </c>
       <c r="C4" s="17">
-        <v>15.600000000000001</v>
+        <v>54.974400000000003</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="20"/>
+        <v>112</v>
+      </c>
       <c r="K4" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="18">
-        <f t="shared" si="0"/>
-        <v>43405</v>
-      </c>
-      <c r="C5" s="17">
-        <v>54.974400000000003</v>
-      </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="K5" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="18">
-        <f t="shared" si="0"/>
-        <v>43405</v>
-      </c>
-      <c r="C6" s="17">
-        <v>156</v>
-      </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="K6" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="18">
-        <f t="shared" si="0"/>
-        <v>43405</v>
-      </c>
-      <c r="C7" s="17">
-        <v>3.1044</v>
-      </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="K7" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="18">
-        <f t="shared" si="0"/>
-        <v>43405</v>
-      </c>
-      <c r="C8" s="17">
-        <v>3.1044</v>
-      </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="K8" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="18">
-        <f t="shared" si="0"/>
-        <v>43405</v>
-      </c>
-      <c r="C9" s="17">
-        <v>90.22</v>
-      </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="K9" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="18">
-        <f t="shared" si="0"/>
-        <v>43405</v>
-      </c>
-      <c r="C10" s="17">
-        <v>78</v>
-      </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="K10" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="18">
-        <f>$J$3+K11</f>
-        <v>43405</v>
-      </c>
-      <c r="C11" s="17">
-        <v>120.83759999999999</v>
-      </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="K11" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F12" s="14"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="49" t="s">
+        <v>109</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1626,14 +1489,14 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
@@ -1642,7 +1505,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="34" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B1" s="34" t="s">
         <v>1</v>
@@ -1658,16 +1521,16 @@
         <v>3</v>
       </c>
       <c r="G1" s="34" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="H1" s="34"/>
       <c r="I1" s="34" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="34" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="17"/>
@@ -1675,7 +1538,7 @@
     </row>
     <row r="3" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B3" s="18">
         <f>$K$3+L3</f>
@@ -1688,54 +1551,54 @@
         <v>19</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="K3" s="20"/>
     </row>
     <row r="4" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B4" s="18">
         <f>$K$3+L4</f>
         <v>0</v>
       </c>
       <c r="C4" s="17">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="K4" s="20"/>
     </row>
     <row r="5" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="B5" s="18">
         <f>$K$3+L5</f>
         <v>0</v>
       </c>
       <c r="C5" s="17">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E5" s="19" t="s">
         <v>19</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="16" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="C6" s="48">
         <f>SUM(C3:C5)</f>
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
@@ -1750,7 +1613,7 @@
     </row>
     <row r="8" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="15" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="17"/>
@@ -1759,23 +1622,23 @@
     </row>
     <row r="9" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="B9" s="18">
         <f>$K$9+L9</f>
-        <v>43405</v>
+        <v>43617</v>
       </c>
       <c r="C9" s="17">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E9" s="19" t="s">
         <v>19</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K9" s="20">
-        <v>43404</v>
+        <v>43616</v>
       </c>
       <c r="L9" s="14">
         <v>1</v>
@@ -1783,20 +1646,20 @@
     </row>
     <row r="10" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="B10" s="18">
         <f t="shared" ref="B10:B11" si="0">$K$9+L10</f>
-        <v>43406</v>
+        <v>43618</v>
       </c>
       <c r="C10" s="17">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K10" s="20"/>
       <c r="L10" s="14">
@@ -1805,20 +1668,20 @@
     </row>
     <row r="11" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="B11" s="18">
         <f t="shared" si="0"/>
-        <v>43407</v>
+        <v>43619</v>
       </c>
       <c r="C11" s="17">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>19</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L11" s="14">
         <v>3</v>
@@ -1826,7 +1689,7 @@
     </row>
     <row r="12" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B12" s="46" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="17"/>
@@ -1835,20 +1698,17 @@
     </row>
     <row r="13" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="B13" s="18">
         <f>$K$9+L13</f>
-        <v>43405</v>
+        <v>43617</v>
       </c>
       <c r="C13" s="17">
-        <v>35</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>96</v>
+        <v>65</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>83</v>
       </c>
       <c r="L13" s="14">
         <v>1</v>
@@ -1856,20 +1716,17 @@
     </row>
     <row r="14" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="B14" s="18">
         <f t="shared" ref="B14:B15" si="1">$K$9+L14</f>
-        <v>43406</v>
+        <v>43618</v>
       </c>
       <c r="C14" s="17">
-        <v>40</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>97</v>
+        <v>75</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>84</v>
       </c>
       <c r="L14" s="14">
         <v>2</v>
@@ -1877,20 +1734,17 @@
     </row>
     <row r="15" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="B15" s="18">
         <f t="shared" si="1"/>
-        <v>43407</v>
+        <v>43619</v>
       </c>
       <c r="C15" s="17">
-        <v>45</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>98</v>
+        <v>85</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>85</v>
       </c>
       <c r="L15" s="14">
         <v>3</v>
@@ -1898,28 +1752,26 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" s="46" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="B17" s="18">
         <f>$K$9+L17</f>
-        <v>43405</v>
+        <v>43617</v>
       </c>
       <c r="C17" s="17">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="D17" s="14"/>
-      <c r="E17" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>93</v>
-      </c>
+      <c r="E17" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F17" s="14"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
@@ -1931,22 +1783,20 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="B18" s="18">
         <f t="shared" ref="B18:B19" si="2">$K$9+L18</f>
-        <v>43406</v>
+        <v>43618</v>
       </c>
       <c r="C18" s="17">
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="D18" s="14"/>
-      <c r="E18" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>94</v>
-      </c>
+      <c r="E18" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="14"/>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
@@ -1958,22 +1808,20 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="B19" s="18">
         <f t="shared" si="2"/>
-        <v>43407</v>
+        <v>43619</v>
       </c>
       <c r="C19" s="17">
-        <v>60</v>
+        <v>115</v>
       </c>
       <c r="D19" s="14"/>
-      <c r="E19" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>95</v>
-      </c>
+      <c r="E19" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" s="14"/>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
@@ -1985,11 +1833,11 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B20" s="45" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="C20" s="12">
         <f>SUM(C9:C19)</f>
-        <v>360</v>
+        <v>675</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1997,25 +1845,25 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B22" s="34" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="B23" s="18">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="C23" s="17">
-        <v>65</v>
+        <v>125</v>
       </c>
       <c r="D23" s="14"/>
       <c r="E23" s="19" t="s">
         <v>19</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
@@ -2026,20 +1874,20 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="B24" s="18">
-        <v>43191</v>
+        <v>43647</v>
       </c>
       <c r="C24" s="17">
-        <v>70</v>
+        <v>135</v>
       </c>
       <c r="D24" s="14"/>
       <c r="E24" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
@@ -2050,20 +1898,20 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="B25" s="18">
-        <v>43405</v>
+        <v>43770</v>
       </c>
       <c r="C25" s="17">
-        <v>75</v>
+        <v>145</v>
       </c>
       <c r="D25" s="14"/>
       <c r="E25" s="19" t="s">
         <v>19</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
@@ -2074,11 +1922,11 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B26" s="47" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="C26" s="12">
         <f>SUM(C23:C25)</f>
-        <v>210</v>
+        <v>405</v>
       </c>
     </row>
   </sheetData>
@@ -2089,11 +1937,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C703CDFE-5895-4A70-B218-454B4A08CC66}">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2:G4"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2130,17 +1978,17 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>43374</v>
+        <v>43586</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="29" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="13">
@@ -2149,32 +1997,32 @@
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
-      <c r="L2" s="30">
-        <v>43374</v>
+      <c r="L2" s="5">
+        <v>43586</v>
       </c>
       <c r="M2">
         <v>5</v>
       </c>
       <c r="N2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="O2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>43375</v>
+        <v>43587</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3" s="29" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="F3" s="10"/>
       <c r="G3" s="13">
@@ -2183,32 +2031,32 @@
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
-      <c r="L3" s="30">
-        <v>43740</v>
+      <c r="L3" s="5">
+        <v>43587</v>
       </c>
       <c r="M3">
         <v>10</v>
       </c>
       <c r="N3" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="O3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>43376</v>
+        <v>43588</v>
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="29" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="F4" s="10">
         <v>12345</v>
@@ -2219,43 +2067,111 @@
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
-      <c r="L4" s="30">
-        <v>43741</v>
+      <c r="L4" s="5">
+        <v>43588</v>
       </c>
       <c r="M4">
         <v>15</v>
       </c>
       <c r="N4" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="O4" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
-        <v>9</v>
+      <c r="A5" s="5">
+        <v>43597</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="13">
+        <v>500</v>
+      </c>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="L5" s="5">
+        <v>43597</v>
+      </c>
+      <c r="M5">
+        <v>500</v>
+      </c>
+      <c r="N5" t="s">
+        <v>46</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>43404</v>
-      </c>
-      <c r="B6" s="13">
-        <v>5.05</v>
-      </c>
-      <c r="C6" s="13"/>
+        <v>43598</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="29" t="s">
+        <v>44</v>
+      </c>
       <c r="D6" s="7" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>54</v>
+        <v>120</v>
       </c>
       <c r="F6" s="10"/>
-      <c r="G6" s="13"/>
+      <c r="G6" s="13">
+        <v>1500</v>
+      </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
+      <c r="L6" s="5">
+        <v>43598</v>
+      </c>
+      <c r="M6">
+        <v>1500</v>
+      </c>
+      <c r="N6" t="s">
+        <v>46</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>43616</v>
+      </c>
+      <c r="B8" s="13">
+        <v>5.05</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2265,11 +2181,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D874970E-DFC7-41AF-9C75-179A4BAE8469}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2288,89 +2204,89 @@
         <v>1</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C1" s="33"/>
       <c r="D1" s="34" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="F1" s="34" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>43374</v>
+        <v>43586</v>
       </c>
       <c r="B2" s="37"/>
       <c r="C2" s="29" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E2" s="13">
         <v>5</v>
       </c>
-      <c r="H2" s="30">
-        <v>43374</v>
+      <c r="H2" s="5">
+        <v>43586</v>
       </c>
       <c r="I2">
         <v>5</v>
       </c>
       <c r="J2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>43740</v>
+        <v>43587</v>
       </c>
       <c r="B3" s="37"/>
       <c r="C3" s="29" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E3" s="13">
         <v>10</v>
       </c>
-      <c r="H3" s="30">
-        <v>43740</v>
+      <c r="H3" s="5">
+        <v>43587</v>
       </c>
       <c r="I3">
         <v>10</v>
       </c>
       <c r="J3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>43741</v>
+        <v>43588</v>
       </c>
       <c r="B4" s="37"/>
       <c r="C4" s="29" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E4" s="13">
         <v>15</v>
       </c>
-      <c r="H4" s="30">
-        <v>43741</v>
+      <c r="H4" s="5">
+        <v>43588</v>
       </c>
       <c r="I4">
         <v>15</v>
       </c>
       <c r="J4" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2381,27 +2297,15 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>43404</v>
+        <v>43616</v>
       </c>
       <c r="B6" s="37">
         <v>10</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E6" s="13"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="37"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="13"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="37"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2411,11 +2315,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A79CC3C-10DD-4C9D-955D-781259440CED}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2434,89 +2338,89 @@
         <v>1</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C1" s="33"/>
       <c r="D1" s="34" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="F1" s="34" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>43374</v>
+        <v>43586</v>
       </c>
       <c r="B2" s="37"/>
       <c r="C2" s="29" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E2" s="13">
         <v>5</v>
       </c>
-      <c r="H2" s="30">
-        <v>43374</v>
+      <c r="H2" s="5">
+        <v>43586</v>
       </c>
       <c r="I2">
         <v>5</v>
       </c>
       <c r="J2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>43740</v>
+        <v>43587</v>
       </c>
       <c r="B3" s="37"/>
       <c r="C3" s="29" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E3" s="13">
         <v>10</v>
       </c>
-      <c r="H3" s="30">
-        <v>43740</v>
+      <c r="H3" s="5">
+        <v>43587</v>
       </c>
       <c r="I3">
         <v>10</v>
       </c>
       <c r="J3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>43741</v>
+        <v>43588</v>
       </c>
       <c r="B4" s="37"/>
       <c r="C4" s="29" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E4" s="13">
         <v>15</v>
       </c>
-      <c r="H4" s="30">
-        <v>43741</v>
+      <c r="H4" s="5">
+        <v>43588</v>
       </c>
       <c r="I4">
         <v>15</v>
       </c>
       <c r="J4" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2527,27 +2431,15 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>43404</v>
+        <v>43616</v>
       </c>
       <c r="B6" s="37">
         <v>10</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E6" s="13"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="37"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="13"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="37"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2561,7 +2453,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2580,31 +2472,31 @@
         <v>1</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D1" s="36" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E1" s="32" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="G1" s="34" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="39"/>
       <c r="I1" s="34" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="30">
-        <v>43374</v>
+      <c r="A2" s="5">
+        <v>43586</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>11</v>
@@ -2612,16 +2504,16 @@
       <c r="D2" s="38">
         <v>5</v>
       </c>
-      <c r="E2" s="30">
-        <v>43374</v>
+      <c r="E2" s="5">
+        <v>43586</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="30">
-        <v>43375</v>
+      <c r="A3" s="5">
+        <v>43587</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>11</v>
@@ -2629,19 +2521,19 @@
       <c r="D3" s="38">
         <v>10</v>
       </c>
-      <c r="E3" s="30">
-        <v>43375</v>
+      <c r="E3" s="5">
+        <v>43587</v>
       </c>
       <c r="F3" s="38">
         <v>25</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="30">
-        <v>43376</v>
+      <c r="A4" s="5">
+        <v>43588</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>12</v>
@@ -2649,14 +2541,14 @@
       <c r="D4" s="38">
         <v>15</v>
       </c>
-      <c r="E4" s="30">
-        <v>43375</v>
+      <c r="E4" s="5">
+        <v>43588</v>
       </c>
       <c r="F4" s="38">
         <v>25</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2665,45 +2557,45 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="30">
-        <v>43405</v>
+      <c r="A6" s="5">
+        <v>43617</v>
       </c>
       <c r="B6" s="38">
         <v>20</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="30">
-        <v>43406</v>
+      <c r="A7" s="5">
+        <v>43618</v>
       </c>
       <c r="B7" s="38">
         <v>25</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="30">
-        <v>43407</v>
+      <c r="A8" s="5">
+        <v>43619</v>
       </c>
       <c r="B8" s="38">
         <v>30</v>
       </c>
       <c r="C8" s="40" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2717,7 +2609,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2730,15 +2622,15 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B1" s="22">
-        <f>SUM(B2:B295)</f>
+        <f>SUM(B2:B287)</f>
         <v>9665.7950000000001</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E1" s="24"/>
       <c r="F1" s="23"/>
@@ -2755,7 +2647,7 @@
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E2" s="27"/>
       <c r="F2" s="26"/>
@@ -2768,7 +2660,7 @@
       <c r="B3" s="25"/>
       <c r="C3" s="26"/>
       <c r="D3" s="28" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E3" s="27"/>
       <c r="F3" s="26"/>
@@ -2785,7 +2677,7 @@
       </c>
       <c r="C4" s="26"/>
       <c r="D4" s="26" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="26"/>
@@ -2802,7 +2694,7 @@
       </c>
       <c r="C5" s="26"/>
       <c r="D5" s="28" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="26"/>
@@ -2815,7 +2707,7 @@
       <c r="B6" s="25"/>
       <c r="C6" s="26"/>
       <c r="D6" s="28" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E6" s="27"/>
       <c r="F6" s="26"/>
@@ -2830,7 +2722,7 @@
       </c>
       <c r="C7" s="26"/>
       <c r="D7" s="28" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E7" s="27"/>
       <c r="F7" s="26"/>
@@ -2845,7 +2737,7 @@
       </c>
       <c r="C8" s="26"/>
       <c r="D8" s="28" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E8" s="27"/>
       <c r="F8" s="26"/>
@@ -2862,7 +2754,7 @@
       </c>
       <c r="C9" s="26"/>
       <c r="D9" s="28" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="E9" s="27"/>
       <c r="F9" s="26"/>
@@ -2877,7 +2769,7 @@
       </c>
       <c r="C10" s="26"/>
       <c r="D10" s="28" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="E10" s="27"/>
       <c r="F10" s="26"/>
@@ -2894,7 +2786,7 @@
       </c>
       <c r="C11" s="26"/>
       <c r="D11" s="28" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="E11" s="27"/>
       <c r="F11" s="26"/>
@@ -2905,13 +2797,13 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="21"/>
       <c r="B12" s="23" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E12" s="24"/>
       <c r="F12" s="23"/>
@@ -2928,7 +2820,7 @@
       </c>
       <c r="C13" s="26"/>
       <c r="D13" s="28" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="G13" s="26"/>
       <c r="H13" s="26"/>
@@ -2943,7 +2835,7 @@
       </c>
       <c r="C14" s="26"/>
       <c r="D14" s="28" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E14" s="27"/>
       <c r="F14" s="26"/>
@@ -2954,13 +2846,13 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="21"/>
       <c r="B15" s="23" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E15" s="24"/>
       <c r="F15" s="23"/>
@@ -2977,7 +2869,7 @@
       </c>
       <c r="C16" s="23"/>
       <c r="D16" s="28" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E16" s="24"/>
       <c r="F16" s="23"/>
@@ -2994,7 +2886,7 @@
       </c>
       <c r="C17" s="23"/>
       <c r="D17" s="28" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="E17" s="24"/>
       <c r="F17" s="23"/>
@@ -3004,14 +2896,14 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B18" s="25">
         <v>1265.2239999999999</v>
       </c>
       <c r="C18" s="26"/>
       <c r="D18" s="28" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E18" s="27"/>
       <c r="F18" s="26"/>
@@ -3021,14 +2913,14 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B19" s="25">
         <v>2633.3320000000003</v>
       </c>
       <c r="C19" s="26"/>
       <c r="D19" s="28" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E19" s="27"/>
       <c r="F19" s="26"/>
@@ -3044,7 +2936,7 @@
         <v>2633.3320000000003</v>
       </c>
       <c r="D20" s="28" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="E20" s="27"/>
       <c r="F20" s="26"/>
@@ -3062,8 +2954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F099FAD4-8B8D-4D3B-8EA7-219D6B3E3C24}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3088,12 +2980,12 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B2" s="41"/>
       <c r="C2" s="7"/>
       <c r="D2" s="34" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="7"/>
@@ -3108,38 +3000,38 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B4" s="41">
-        <v>12081.55</v>
+        <v>1000</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E4" s="13">
         <v>-1000</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D5" s="7" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="E5" s="13">
         <v>-1000</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>75</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D6" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="E6" s="13">
         <v>-1000</v>
@@ -3148,13 +3040,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D7" s="7" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E7" s="13">
         <v>-1000</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>74</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -3168,7 +3060,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3185,29 +3077,29 @@
         <v>1</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C1" s="33"/>
       <c r="D1" s="34" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="44" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="F1" s="34" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>43374</v>
+        <v>43586</v>
       </c>
       <c r="B2" s="37"/>
       <c r="C2" s="29" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E2" s="37">
         <v>5</v>
@@ -3215,14 +3107,14 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>43375</v>
+        <v>43587</v>
       </c>
       <c r="B3" s="37"/>
       <c r="C3" s="29" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E3" s="37">
         <v>10</v>
@@ -3230,14 +3122,14 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>43376</v>
+        <v>43588</v>
       </c>
       <c r="B4" s="37"/>
       <c r="C4" s="29" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E4" s="37">
         <v>15</v>
@@ -3245,13 +3137,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="30">
-        <v>43405</v>
+        <v>43617</v>
       </c>
       <c r="B5" s="38">
         <v>20</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -3265,7 +3157,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3279,7 +3171,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="43" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="C1" s="43" t="s">
         <v>8</v>
@@ -3287,7 +3179,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="30">
-        <v>43313</v>
+        <v>43525</v>
       </c>
       <c r="B2" s="38">
         <v>100</v>
@@ -3298,7 +3190,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="30">
-        <v>43344</v>
+        <v>43556</v>
       </c>
       <c r="B3" s="38">
         <v>100</v>
@@ -3309,7 +3201,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="30">
-        <v>43374</v>
+        <v>43586</v>
       </c>
       <c r="B4" s="38">
         <v>100</v>

</xml_diff>

<commit_message>
Added mortgage rows to Budget Out and Bank Out sheets in sample spreadsheet
</commit_message>
<xml_diff>
--- a/reconciliation-samples/For debugging/Your-Spreadsheet.xlsx
+++ b/reconciliation-samples/For debugging/Your-Spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\reconciliation-samples\For debugging\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/csudbery/ReconciliateCsvs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4EDA34A-CEDC-43DA-A544-2296E755994D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC415C8-4329-A84C-BBD6-0F7DE871DFDE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
+    <workbookView xWindow="25680" yWindow="8980" windowWidth="25600" windowHeight="8940" activeTab="10" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Bank In" sheetId="7" r:id="rId1"/>
@@ -257,7 +257,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="123">
   <si>
     <t>notes</t>
   </si>
@@ -577,9 +577,6 @@
     <t>!! ActualBank bal !!</t>
   </si>
   <si>
-    <t>CRED CARD 2</t>
-  </si>
-  <si>
     <t>"CRED CARD 2"</t>
   </si>
   <si>
@@ -620,6 +617,15 @@
   </si>
   <si>
     <t>CREDIT CARD 2</t>
+  </si>
+  <si>
+    <t>Code042</t>
+  </si>
+  <si>
+    <t>Mortgage description</t>
+  </si>
+  <si>
+    <t>"Mortgage description"</t>
   </si>
 </sst>
 </file>
@@ -627,8 +633,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
-    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00_);[Red]\(&quot;£&quot;#,##0.00\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00_);[Red]\(&quot;£&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="166" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
@@ -704,18 +710,18 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -723,7 +729,7 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -734,10 +740,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -747,30 +753,30 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1197,19 +1203,19 @@
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="1.85546875" customWidth="1"/>
-    <col min="5" max="5" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.83203125" customWidth="1"/>
+    <col min="5" max="5" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" style="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1229,7 +1235,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>43586</v>
       </c>
@@ -1263,7 +1269,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>43587</v>
       </c>
@@ -1297,7 +1303,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>43588</v>
       </c>
@@ -1333,13 +1339,13 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B5" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="12"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>43616</v>
       </c>
@@ -1374,15 +1380,15 @@
       <selection pane="bottomLeft" activeCell="F2" sqref="F2:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="45" t="s">
         <v>21</v>
       </c>
@@ -1403,7 +1409,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
         <v>10</v>
       </c>
@@ -1419,7 +1425,7 @@
         <v>19</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J2" s="20">
         <v>43616</v>
@@ -1428,7 +1434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
         <v>11</v>
       </c>
@@ -1444,14 +1450,14 @@
         <v>20</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J3" s="20"/>
       <c r="K3" s="14">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
         <v>12</v>
       </c>
@@ -1467,15 +1473,15 @@
         <v>19</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K4" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" s="49" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1485,25 +1491,25 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FF22F54-1C2B-49C1-90A9-21044AC295B0}">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="34" t="s">
         <v>21</v>
       </c>
@@ -1528,7 +1534,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="34" t="s">
         <v>72</v>
       </c>
@@ -1536,7 +1542,7 @@
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
     </row>
-    <row r="3" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
         <v>26</v>
       </c>
@@ -1555,7 +1561,7 @@
       </c>
       <c r="K3" s="20"/>
     </row>
-    <row r="4" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
         <v>27</v>
       </c>
@@ -1574,7 +1580,7 @@
       </c>
       <c r="K4" s="20"/>
     </row>
-    <row r="5" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="14" t="s">
         <v>86</v>
       </c>
@@ -1592,7 +1598,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="16" t="s">
         <v>73</v>
       </c>
@@ -1604,14 +1610,14 @@
       <c r="E6" s="17"/>
       <c r="F6" s="19"/>
     </row>
-    <row r="7" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="16"/>
       <c r="C7" s="18"/>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
       <c r="F7" s="19"/>
     </row>
-    <row r="8" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="15" t="s">
         <v>74</v>
       </c>
@@ -1620,7 +1626,7 @@
       <c r="E8" s="17"/>
       <c r="F8" s="19"/>
     </row>
-    <row r="9" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>87</v>
       </c>
@@ -1635,7 +1641,7 @@
         <v>19</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K9" s="20">
         <v>43616</v>
@@ -1644,12 +1650,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="14" t="s">
         <v>88</v>
       </c>
       <c r="B10" s="18">
-        <f t="shared" ref="B10:B11" si="0">$K$9+L10</f>
+        <f t="shared" ref="B10:B12" si="0">$K$9+L10</f>
         <v>43618</v>
       </c>
       <c r="C10" s="17">
@@ -1659,14 +1665,14 @@
         <v>20</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K10" s="20"/>
       <c r="L10" s="14">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="14" t="s">
         <v>89</v>
       </c>
@@ -1681,120 +1687,116 @@
         <v>19</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L11" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B12" s="46" t="s">
+    <row r="12" spans="1:12" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B12" s="18">
+        <f t="shared" si="0"/>
+        <v>43620</v>
+      </c>
+      <c r="C12" s="17">
+        <v>1000</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="L12" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="B13" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="19"/>
-    </row>
-    <row r="13" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="14" t="s">
+      <c r="C13" s="18"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="19"/>
+    </row>
+    <row r="14" spans="1:12" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A14" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="B13" s="18">
-        <f>$K$9+L13</f>
+      <c r="B14" s="18">
+        <f>$K$9+L14</f>
         <v>43617</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C14" s="17">
         <v>65</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E14" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="L13" s="14">
+      <c r="L14" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
+    <row r="15" spans="1:12" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A15" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="18">
-        <f t="shared" ref="B14:B15" si="1">$K$9+L14</f>
+      <c r="B15" s="18">
+        <f t="shared" ref="B15:B16" si="1">$K$9+L15</f>
         <v>43618</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C15" s="17">
         <v>75</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E15" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="L14" s="14">
+      <c r="L15" s="14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="14" t="s">
+    <row r="16" spans="1:12" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A16" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="B15" s="18">
+      <c r="B16" s="18">
         <f t="shared" si="1"/>
         <v>43619</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C16" s="17">
         <v>85</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E16" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="L15" s="14">
+      <c r="L16" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="46" t="s">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B17" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="G16" s="14"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B17" s="18">
-        <f>$K$9+L17</f>
+      <c r="B18" s="18">
+        <f>$K$9+L18</f>
         <v>43617</v>
       </c>
-      <c r="C17" s="17">
+      <c r="C18" s="17">
         <v>95</v>
-      </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="B18" s="18">
-        <f t="shared" ref="B18:B19" si="2">$K$9+L18</f>
-        <v>43618</v>
-      </c>
-      <c r="C18" s="17">
-        <v>105</v>
       </c>
       <c r="D18" s="14"/>
       <c r="E18" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
@@ -1803,91 +1805,92 @@
       <c r="J18" s="14"/>
       <c r="K18" s="20"/>
       <c r="L18" s="14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B19" s="18">
-        <f t="shared" si="2"/>
-        <v>43619</v>
+        <f t="shared" ref="B19:B20" si="2">$K$9+L19</f>
+        <v>43618</v>
       </c>
       <c r="C19" s="17">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="D19" s="14"/>
       <c r="E19" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
+      <c r="K19" s="20"/>
       <c r="L19" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" s="18">
+        <f t="shared" si="2"/>
+        <v>43619</v>
+      </c>
+      <c r="C20" s="17">
+        <v>115</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="45" t="s">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B21" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="C20" s="12">
-        <f>SUM(C9:C19)</f>
-        <v>675</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="7"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="34" t="s">
+      <c r="C21" s="12">
+        <f>SUM(C9:C20)</f>
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B22" s="7"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B23" s="34" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="B23" s="18">
+      <c r="B24" s="18">
         <v>43466</v>
       </c>
-      <c r="C23" s="17">
+      <c r="C24" s="17">
         <v>125</v>
-      </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="14"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="B24" s="18">
-        <v>43647</v>
-      </c>
-      <c r="C24" s="17">
-        <v>135</v>
       </c>
       <c r="D24" s="14"/>
       <c r="E24" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
@@ -1896,36 +1899,60 @@
       <c r="K24" s="20"/>
       <c r="L24" s="14"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B25" s="18">
-        <v>43770</v>
+        <v>43647</v>
       </c>
       <c r="C25" s="17">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D25" s="14"/>
       <c r="E25" s="19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
       <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
+      <c r="K25" s="20"/>
       <c r="L25" s="14"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="47" t="s">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" s="18">
+        <v>43770</v>
+      </c>
+      <c r="C26" s="17">
+        <v>145</v>
+      </c>
+      <c r="D26" s="14"/>
+      <c r="E26" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B27" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="C26" s="12">
-        <f>SUM(C23:C25)</f>
+      <c r="C27" s="12">
+        <f>SUM(C24:C26)</f>
         <v>405</v>
       </c>
     </row>
@@ -1937,26 +1964,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C703CDFE-5895-4A70-B218-454B4A08CC66}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="1.85546875" customWidth="1"/>
-    <col min="5" max="5" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.83203125" customWidth="1"/>
+    <col min="5" max="5" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" style="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1976,7 +2003,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>43586</v>
       </c>
@@ -2010,7 +2037,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>43587</v>
       </c>
@@ -2044,7 +2071,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>43588</v>
       </c>
@@ -2080,9 +2107,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
-        <v>43597</v>
+        <v>43589</v>
       </c>
       <c r="B5" s="13"/>
       <c r="C5" s="29" t="s">
@@ -2091,32 +2118,32 @@
       <c r="D5" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>119</v>
+      <c r="E5" s="14" t="s">
+        <v>121</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="13">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="L5" s="5">
-        <v>43597</v>
+        <v>43589</v>
       </c>
       <c r="M5">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="N5" t="s">
         <v>46</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
-        <v>43598</v>
+        <v>43597</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="29" t="s">
@@ -2126,20 +2153,20 @@
         <v>43</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="13">
-        <v>1500</v>
+        <v>500</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="L6" s="5">
-        <v>43598</v>
+        <v>43597</v>
       </c>
       <c r="M6">
-        <v>1500</v>
+        <v>500</v>
       </c>
       <c r="N6" t="s">
         <v>46</v>
@@ -2148,30 +2175,64 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="12" t="s">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>43598</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="13">
+        <v>1500</v>
+      </c>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="L7" s="5">
+        <v>43598</v>
+      </c>
+      <c r="M7">
+        <v>1500</v>
+      </c>
+      <c r="N7" t="s">
+        <v>46</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B8" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
         <v>43616</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B9" s="13">
         <v>5.05</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="7" t="s">
+      <c r="C9" s="13"/>
+      <c r="D9" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E9" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2185,21 +2246,21 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.140625" customWidth="1"/>
-    <col min="4" max="4" width="30.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.1640625" customWidth="1"/>
+    <col min="4" max="4" width="30.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
         <v>1</v>
       </c>
@@ -2217,7 +2278,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>43586</v>
       </c>
@@ -2241,7 +2302,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>43587</v>
       </c>
@@ -2265,7 +2326,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>43588</v>
       </c>
@@ -2289,13 +2350,13 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5" s="38" t="s">
         <v>9</v>
       </c>
       <c r="D5"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>43616</v>
       </c>
@@ -2322,18 +2383,18 @@
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.140625" customWidth="1"/>
-    <col min="4" max="4" width="30.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.1640625" customWidth="1"/>
+    <col min="4" max="4" width="30.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
         <v>1</v>
       </c>
@@ -2351,7 +2412,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>43586</v>
       </c>
@@ -2375,7 +2436,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>43587</v>
       </c>
@@ -2399,7 +2460,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>43588</v>
       </c>
@@ -2423,13 +2484,13 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5" s="38" t="s">
         <v>9</v>
       </c>
       <c r="D5"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>43616</v>
       </c>
@@ -2453,21 +2514,21 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6:A8"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" style="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="38" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="38" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5" style="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" style="38" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" style="38" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="34" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="34" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="32" t="s">
         <v>1</v>
       </c>
@@ -2494,7 +2555,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>43586</v>
       </c>
@@ -2511,7 +2572,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>43587</v>
       </c>
@@ -2531,7 +2592,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>43588</v>
       </c>
@@ -2551,12 +2612,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" s="37" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>43617</v>
       </c>
@@ -2570,7 +2631,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>43618</v>
       </c>
@@ -2584,7 +2645,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>43619</v>
       </c>
@@ -2608,19 +2669,19 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21:XFD28"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>21</v>
       </c>
@@ -2638,7 +2699,7 @@
       <c r="H1" s="23"/>
       <c r="I1" s="23"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
@@ -2655,7 +2716,7 @@
       <c r="H2" s="26"/>
       <c r="I2" s="26"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="28"/>
       <c r="B3" s="25"/>
       <c r="C3" s="26"/>
@@ -2668,7 +2729,7 @@
       <c r="H3" s="26"/>
       <c r="I3" s="26"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>11</v>
       </c>
@@ -2685,7 +2746,7 @@
       <c r="H4" s="26"/>
       <c r="I4" s="26"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>12</v>
       </c>
@@ -2702,7 +2763,7 @@
       <c r="H5" s="26"/>
       <c r="I5" s="26"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="28"/>
       <c r="B6" s="25"/>
       <c r="C6" s="26"/>
@@ -2715,7 +2776,7 @@
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="28"/>
       <c r="B7" s="25">
         <v>534</v>
@@ -2730,7 +2791,7 @@
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="28"/>
       <c r="B8" s="25">
         <v>70.31</v>
@@ -2745,7 +2806,7 @@
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
         <v>13</v>
       </c>
@@ -2762,7 +2823,7 @@
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="28"/>
       <c r="B10" s="25">
         <v>168.21</v>
@@ -2777,7 +2838,7 @@
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
         <v>14</v>
       </c>
@@ -2794,7 +2855,7 @@
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="21"/>
       <c r="B12" s="23" t="s">
         <v>23</v>
@@ -2811,7 +2872,7 @@
       <c r="H12" s="23"/>
       <c r="I12" s="23"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
         <v>15</v>
       </c>
@@ -2826,7 +2887,7 @@
       <c r="H13" s="26"/>
       <c r="I13" s="26"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
         <v>16</v>
       </c>
@@ -2843,7 +2904,7 @@
       <c r="H14" s="26"/>
       <c r="I14" s="26"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="21"/>
       <c r="B15" s="23" t="s">
         <v>23</v>
@@ -2860,7 +2921,7 @@
       <c r="H15" s="23"/>
       <c r="I15" s="23"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
         <v>17</v>
       </c>
@@ -2877,7 +2938,7 @@
       <c r="H16" s="23"/>
       <c r="I16" s="23"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
         <v>18</v>
       </c>
@@ -2894,7 +2955,7 @@
       <c r="H17" s="23"/>
       <c r="I17" s="23"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="19" t="s">
         <v>26</v>
       </c>
@@ -2911,7 +2972,7 @@
       <c r="H18" s="26"/>
       <c r="I18" s="26"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
         <v>27</v>
       </c>
@@ -2928,7 +2989,7 @@
       <c r="H19" s="26"/>
       <c r="I19" s="26"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="28"/>
       <c r="B20" s="25"/>
       <c r="C20" s="25">
@@ -2958,17 +3019,17 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="91.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="91.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="7"/>
       <c r="B1" s="41"/>
       <c r="C1" s="7"/>
@@ -2978,7 +3039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="34" t="s">
         <v>60</v>
       </c>
@@ -2990,7 +3051,7 @@
       <c r="E2" s="13"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="34"/>
       <c r="B3" s="41"/>
       <c r="C3" s="7"/>
@@ -2998,7 +3059,7 @@
       <c r="E3" s="13"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>62</v>
       </c>
@@ -3015,10 +3076,10 @@
         <v>-1000</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D5" s="7" t="s">
         <v>64</v>
       </c>
@@ -3026,10 +3087,10 @@
         <v>-1000</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D6" s="7" t="s">
         <v>65</v>
       </c>
@@ -3038,7 +3099,7 @@
       </c>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D7" s="7" t="s">
         <v>66</v>
       </c>
@@ -3046,7 +3107,7 @@
         <v>-1000</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -3063,16 +3124,16 @@
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" style="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.42578125" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5" style="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.5" customWidth="1"/>
+    <col min="4" max="4" width="34.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="38" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
         <v>1</v>
       </c>
@@ -3090,7 +3151,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>43586</v>
       </c>
@@ -3105,7 +3166,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>43587</v>
       </c>
@@ -3120,7 +3181,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>43588</v>
       </c>
@@ -3135,7 +3196,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="30">
         <v>43617</v>
       </c>
@@ -3160,13 +3221,13 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.140625" style="38"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.1640625" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -3177,7 +3238,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="30">
         <v>43525</v>
       </c>
@@ -3188,7 +3249,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="30">
         <v>43556</v>
       </c>
@@ -3199,7 +3260,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="30">
         <v>43586</v>
       </c>

</xml_diff>